<commit_message>
change vmmc lable (#359)
* change vmmc lable

* fix typo

* change question

Co-authored-by: Emmanuel Amodu <emmanuelamodu@Emmanuels-MacBook-Pro-2.local>
Co-authored-by: femi oni <freefony@gmail.com>
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/day14_no_contact.xlsx
+++ b/config/itech-aurum/forms/app/day14_no_contact.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-93\itech-aurum\forms\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmanuelamodu/Desktop/medic-mobile/config-itech/itech-aurum/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783D893E-C81C-46C8-AF1E-0B123A41B5F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AF6E3C-9B4F-674B-A217-24901BA44B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -184,9 +184,6 @@
     <t>client_ok</t>
   </si>
   <si>
-    <t>Is VMMC Client okay?</t>
-  </si>
-  <si>
     <t>additional_notes_text</t>
   </si>
   <si>
@@ -273,6 +270,9 @@
 &lt;p&gt;2) Client reached and NEEDS in-person review;&lt;/p&gt; 
 &lt;p&gt;3) Client not reached after all attempts and is considered LTFU&lt;/p&gt;&lt;/h4&gt;
 </t>
+  </si>
+  <si>
+    <t>Unknown, Client LTFU</t>
   </si>
 </sst>
 </file>
@@ -759,26 +759,26 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.375" customWidth="1"/>
-    <col min="2" max="2" width="19.125" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
     <col min="3" max="3" width="44" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11.5" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.25" style="45" customWidth="1"/>
+    <col min="9" max="9" width="16.1640625" style="45" customWidth="1"/>
     <col min="10" max="10" width="11.5" customWidth="1"/>
-    <col min="11" max="11" width="29.875" style="45" customWidth="1"/>
+    <col min="11" max="11" width="29.83203125" style="45" customWidth="1"/>
     <col min="12" max="26" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="31.5">
+    <row r="1" spans="1:26" ht="34">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -813,10 +813,10 @@
         <v>10</v>
       </c>
       <c r="L1" s="39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="15.75">
+    <row r="2" spans="1:26" ht="16">
       <c r="A2" s="33" t="s">
         <v>11</v>
       </c>
@@ -841,7 +841,7 @@
       <c r="L2" s="40"/>
       <c r="M2" s="13"/>
     </row>
-    <row r="3" spans="1:26" ht="15.75">
+    <row r="3" spans="1:26" ht="16">
       <c r="A3" s="33" t="s">
         <v>16</v>
       </c>
@@ -866,7 +866,7 @@
       <c r="L3" s="41"/>
       <c r="M3" s="13"/>
     </row>
-    <row r="4" spans="1:26" ht="15.75">
+    <row r="4" spans="1:26" ht="16">
       <c r="A4" s="33" t="s">
         <v>16</v>
       </c>
@@ -889,7 +889,7 @@
       <c r="L4" s="41"/>
       <c r="M4" s="13"/>
     </row>
-    <row r="5" spans="1:26" ht="15.75">
+    <row r="5" spans="1:26" ht="16">
       <c r="A5" s="33" t="s">
         <v>11</v>
       </c>
@@ -910,7 +910,7 @@
       <c r="L5" s="41"/>
       <c r="M5" s="13"/>
     </row>
-    <row r="6" spans="1:26" ht="29.25">
+    <row r="6" spans="1:26" ht="31">
       <c r="A6" s="33" t="s">
         <v>25</v>
       </c>
@@ -937,7 +937,7 @@
       <c r="L6" s="41"/>
       <c r="M6" s="13"/>
     </row>
-    <row r="7" spans="1:26" ht="15.75">
+    <row r="7" spans="1:26" ht="16">
       <c r="A7" s="33" t="s">
         <v>16</v>
       </c>
@@ -960,7 +960,7 @@
       <c r="L7" s="41"/>
       <c r="M7" s="13"/>
     </row>
-    <row r="8" spans="1:26" ht="15.75">
+    <row r="8" spans="1:26" ht="16">
       <c r="A8" s="33" t="s">
         <v>16</v>
       </c>
@@ -983,7 +983,7 @@
       <c r="L8" s="41"/>
       <c r="M8" s="13"/>
     </row>
-    <row r="9" spans="1:26" ht="15.75">
+    <row r="9" spans="1:26" ht="16">
       <c r="A9" s="33" t="s">
         <v>34</v>
       </c>
@@ -1000,7 +1000,7 @@
       <c r="L9" s="41"/>
       <c r="M9" s="13"/>
     </row>
-    <row r="10" spans="1:26" ht="15.75">
+    <row r="10" spans="1:26" ht="16">
       <c r="A10" s="35" t="s">
         <v>34</v>
       </c>
@@ -1017,7 +1017,7 @@
       <c r="L10" s="40"/>
       <c r="M10" s="13"/>
     </row>
-    <row r="11" spans="1:26" ht="15.75">
+    <row r="11" spans="1:26" ht="16">
       <c r="A11" s="37" t="s">
         <v>35</v>
       </c>
@@ -1053,7 +1053,7 @@
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
     </row>
-    <row r="12" spans="1:26" ht="15.75">
+    <row r="12" spans="1:26" ht="16">
       <c r="A12" s="38" t="s">
         <v>35</v>
       </c>
@@ -1093,7 +1093,7 @@
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
     </row>
-    <row r="13" spans="1:26" ht="15.75">
+    <row r="13" spans="1:26" ht="16">
       <c r="A13" s="37" t="s">
         <v>35</v>
       </c>
@@ -1129,7 +1129,7 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:26" ht="15.75">
+    <row r="14" spans="1:26" ht="16">
       <c r="A14" s="27" t="s">
         <v>11</v>
       </c>
@@ -1165,7 +1165,7 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:26" ht="228.75">
+    <row r="15" spans="1:26" ht="226">
       <c r="A15" s="27" t="s">
         <v>45</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>46</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D15" s="24"/>
       <c r="E15" s="24"/>
@@ -1201,7 +1201,7 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:26" ht="15.75">
+    <row r="16" spans="1:26" ht="16">
       <c r="A16" s="27" t="s">
         <v>47</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>48</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="D16" s="24"/>
       <c r="E16" s="24"/>
@@ -1237,25 +1237,25 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" spans="1:26" ht="100.5">
+    <row r="17" spans="1:26" ht="106">
       <c r="A17" s="27" t="s">
         <v>35</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17" s="24"/>
       <c r="D17" s="24"/>
       <c r="E17" s="24"/>
       <c r="F17" s="24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G17" s="24"/>
       <c r="H17" s="24"/>
       <c r="I17" s="44"/>
       <c r="J17" s="24"/>
       <c r="K17" s="44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L17" s="44"/>
       <c r="M17" s="12"/>
@@ -1273,20 +1273,20 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" spans="1:26" ht="15.75">
+    <row r="18" spans="1:26" ht="16">
       <c r="A18" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="C18" s="26" t="s">
         <v>53</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>54</v>
       </c>
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
       <c r="F18" s="24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G18" s="24"/>
       <c r="H18" s="24"/>
@@ -2330,18 +2330,18 @@
       <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="11.5" customWidth="1"/>
-    <col min="3" max="3" width="17.75" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
     <col min="4" max="6" width="11.5" customWidth="1"/>
     <col min="7" max="26" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="16" customFormat="1" ht="15.75">
+    <row r="1" spans="1:3" s="16" customFormat="1" ht="16">
       <c r="A1" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>1</v>
@@ -2357,35 +2357,35 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="A3" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>29</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="A4" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1">
       <c r="A5" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>59</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1">
@@ -3389,43 +3389,43 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.875" customWidth="1"/>
-    <col min="2" max="2" width="43.625" customWidth="1"/>
-    <col min="3" max="3" width="32.875" customWidth="1"/>
-    <col min="4" max="4" width="20.875" customWidth="1"/>
+    <col min="1" max="1" width="31.83203125" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" customWidth="1"/>
+    <col min="3" max="3" width="32.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" customWidth="1"/>
     <col min="5" max="15" width="11.5" customWidth="1"/>
-    <col min="16" max="26" width="8.75" customWidth="1"/>
+    <col min="16" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18" customHeight="1">
       <c r="A1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
@@ -3447,29 +3447,29 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>75</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>76</v>
       </c>
       <c r="C2" s="9">
         <v>43896</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>69</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>70</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>72</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>

</xml_diff>